<commit_message>
rename vaporization_pressure to vapor pressure
</commit_message>
<xml_diff>
--- a/examples/combined.xlsx
+++ b/examples/combined.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GPLCE\code\eEnSa-FocusSteps\Pelmo\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0548DA10-90BA-430F-A3BC-9A38A02B2D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0E22A7-861F-4EE5-8255-4225C6C59347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="10" windowWidth="19180" windowHeight="10060" activeTab="1" xr2:uid="{BABA2AA3-9440-4BC1-BC88-928EBC21D3E0}"/>
+    <workbookView xWindow="14115" yWindow="-15915" windowWidth="25440" windowHeight="15270" xr2:uid="{BABA2AA3-9440-4BC1-BC88-928EBC21D3E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Compound Properties" sheetId="1" r:id="rId1"/>
@@ -77,9 +77,6 @@
     <t>Water Solubility</t>
   </si>
   <si>
-    <t>Vaporization Pressure</t>
-  </si>
-  <si>
     <t>Freundlich</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>Metabolite D2</t>
+  </si>
+  <si>
+    <t>Vapor Pressure</t>
   </si>
 </sst>
 </file>
@@ -614,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98776180-28AB-4EDA-98E2-623B9408684F}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -642,7 +642,7 @@
         <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -651,10 +651,10 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
         <v>13</v>
-      </c>
-      <c r="H1" t="s">
-        <v>14</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -669,12 +669,12 @@
         <v>7</v>
       </c>
       <c r="M1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2">
         <v>1000</v>
@@ -712,7 +712,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3">
         <v>100</v>
@@ -748,12 +748,12 @@
         <v>2</v>
       </c>
       <c r="M3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4">
         <v>100</v>
@@ -789,12 +789,12 @@
         <v>2</v>
       </c>
       <c r="M4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5">
         <v>100</v>
@@ -830,12 +830,12 @@
         <v>2</v>
       </c>
       <c r="M5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6">
         <v>100</v>
@@ -871,12 +871,12 @@
         <v>2</v>
       </c>
       <c r="M6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -912,12 +912,12 @@
         <v>2</v>
       </c>
       <c r="M7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8">
         <v>10</v>
@@ -953,12 +953,12 @@
         <v>2</v>
       </c>
       <c r="M8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9">
         <v>10</v>
@@ -994,12 +994,12 @@
         <v>2</v>
       </c>
       <c r="M9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10">
         <v>10</v>
@@ -1035,7 +1035,7 @@
         <v>2</v>
       </c>
       <c r="M10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
@@ -1072,7 +1072,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04BD9B6D-A104-4391-B639-92AB92087366}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -1097,10 +1097,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
         <v>56</v>
-      </c>
-      <c r="B2" t="s">
-        <v>57</v>
       </c>
       <c r="C2">
         <v>0.1</v>
@@ -1108,10 +1108,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3">
         <v>0.15</v>
@@ -1119,10 +1119,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4">
         <v>0.2</v>
@@ -1130,10 +1130,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5">
         <v>0.25</v>
@@ -1141,10 +1141,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" t="s">
         <v>57</v>
-      </c>
-      <c r="B6" t="s">
-        <v>58</v>
       </c>
       <c r="C6">
         <v>0.1</v>
@@ -1152,10 +1152,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7">
         <v>0.2</v>
@@ -1163,10 +1163,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8">
         <v>0.3</v>
@@ -1174,10 +1174,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" t="s">
         <v>58</v>
-      </c>
-      <c r="B9" t="s">
-        <v>59</v>
       </c>
       <c r="C9">
         <v>0.1</v>
@@ -1185,10 +1185,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10">
         <v>0.2</v>
@@ -1196,10 +1196,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11">
         <v>0.3</v>
@@ -1207,10 +1207,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" t="s">
         <v>59</v>
-      </c>
-      <c r="B12" t="s">
-        <v>60</v>
       </c>
       <c r="C12">
         <v>0.1</v>
@@ -1218,10 +1218,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13">
         <v>0.2</v>
@@ -1229,10 +1229,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14">
         <v>0.3</v>
@@ -1240,10 +1240,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C15">
         <v>0.4</v>
@@ -1251,10 +1251,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" t="s">
         <v>61</v>
-      </c>
-      <c r="B16" t="s">
-        <v>62</v>
       </c>
       <c r="C16">
         <v>0.5</v>
@@ -1262,10 +1262,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" t="s">
         <v>62</v>
-      </c>
-      <c r="B17" t="s">
-        <v>63</v>
       </c>
       <c r="C17">
         <v>0.5</v>
@@ -1273,10 +1273,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" t="s">
         <v>63</v>
-      </c>
-      <c r="B18" t="s">
-        <v>64</v>
       </c>
       <c r="C18">
         <v>0.5</v>
@@ -1300,24 +1300,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>28</v>
-      </c>
-      <c r="E1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -1364,159 +1364,159 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>